<commit_message>
Added iMethodInterceptor to disable test case at run time
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dheer\dj-eclipse-workspace\SeleniumAutomationFramework\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03111934-CBF4-44FE-86C3-DAAD482E9215}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{905C9D2F-6333-45FB-B073-0DD4297B7117}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="testing" sheetId="1" r:id="rId1"/>
+    <sheet name="RUNMANAGER" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
   <si>
     <t>username</t>
   </si>
@@ -70,6 +72,42 @@
   </si>
   <si>
     <t>ngsv</t>
+  </si>
+  <si>
+    <t>testName</t>
+  </si>
+  <si>
+    <t>execute</t>
+  </si>
+  <si>
+    <t>priority</t>
+  </si>
+  <si>
+    <t>count</t>
+  </si>
+  <si>
+    <t>loginLogoutTest</t>
+  </si>
+  <si>
+    <t>Test the login and logout of the app</t>
+  </si>
+  <si>
+    <t>newTest</t>
+  </si>
+  <si>
+    <t>This is second test</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>testDescription</t>
   </si>
 </sst>
 </file>
@@ -105,9 +143,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -390,8 +430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -455,4 +495,131 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9A582ED-5DFC-4F0F-AC91-9D3383FF9CD2}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="14.07421875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.61328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.23046875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A6EB4C6-974F-4107-B561-BDA05CB4B7F6}">
+  <dimension ref="G6:G14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetData>
+    <row r="6" spans="7:7" x14ac:dyDescent="0.4">
+      <c r="G6">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="7" spans="7:7" x14ac:dyDescent="0.4">
+      <c r="G7">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="8" spans="7:7" x14ac:dyDescent="0.4">
+      <c r="G8">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="7:7" x14ac:dyDescent="0.4">
+      <c r="G9">
+        <v>41.25</v>
+      </c>
+    </row>
+    <row r="10" spans="7:7" x14ac:dyDescent="0.4">
+      <c r="G10">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="11" spans="7:7" x14ac:dyDescent="0.4">
+      <c r="G11">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="7:7" x14ac:dyDescent="0.4">
+      <c r="G12">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="14" spans="7:7" x14ac:dyDescent="0.4">
+      <c r="G14">
+        <v>825.25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
implemented DataProvider from excel
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dheer\dj-eclipse-workspace\SeleniumAutomationFramework\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{905C9D2F-6333-45FB-B073-0DD4297B7117}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57732B39-41F0-4CC9-B109-9DB818E8EA19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="testing" sheetId="1" r:id="rId1"/>
+    <sheet name="DATA" sheetId="1" r:id="rId1"/>
     <sheet name="RUNMANAGER" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="27">
   <si>
     <t>username</t>
   </si>
@@ -35,9 +35,6 @@
     <t>password</t>
   </si>
   <si>
-    <t>dhee</t>
-  </si>
-  <si>
     <t>dheeraj</t>
   </si>
   <si>
@@ -47,9 +44,6 @@
     <t>sri</t>
   </si>
   <si>
-    <t>divvu</t>
-  </si>
-  <si>
     <t>div</t>
   </si>
   <si>
@@ -59,18 +53,9 @@
     <t>lastname</t>
   </si>
   <si>
-    <t>123</t>
-  </si>
-  <si>
-    <t>234</t>
-  </si>
-  <si>
     <t>nihan</t>
   </si>
   <si>
-    <t>789</t>
-  </si>
-  <si>
     <t>ngsv</t>
   </si>
   <si>
@@ -108,6 +93,21 @@
   </si>
   <si>
     <t>testDescription</t>
+  </si>
+  <si>
+    <t>testname</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>admin123</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -145,9 +145,9 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -428,68 +428,115 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="14.07421875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" t="s">
         <v>8</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
         <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -501,66 +548,64 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9A582ED-5DFC-4F0F-AC91-9D3383FF9CD2}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="14.07421875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.61328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="9.23046875" style="2"/>
+    <col min="4" max="5" width="9.23046875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>24</v>
+      <c r="D2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>24</v>
+      <c r="D3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -573,7 +618,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A6EB4C6-974F-4107-B561-BDA05CB4B7F6}">
   <dimension ref="G6:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
implemented iRetryAnalyzer and enabled cross browser testing
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dheer\dj-eclipse-workspace\SeleniumAutomationFramework\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57732B39-41F0-4CC9-B109-9DB818E8EA19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0B8DEB5-F88F-4DE0-95EB-AFA60C0810D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="30">
   <si>
     <t>username</t>
   </si>
@@ -108,6 +108,15 @@
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t>browser</t>
+  </si>
+  <si>
+    <t>chrome</t>
+  </si>
+  <si>
+    <t>firefox</t>
   </si>
 </sst>
 </file>
@@ -428,10 +437,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -439,7 +448,7 @@
     <col min="1" max="1" width="14.07421875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -447,19 +456,22 @@
         <v>11</v>
       </c>
       <c r="C1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -467,75 +479,87 @@
         <v>23</v>
       </c>
       <c r="C2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" t="s">
         <v>24</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>25</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>2</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" t="s">
         <v>24</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>25</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>5</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" t="s">
         <v>24</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>25</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>8</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" t="s">
-        <v>25</v>
+        <v>18</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="D5" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="G5" s="3" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>